<commit_message>
Updated the DCF Model
</commit_message>
<xml_diff>
--- a/financial_models/Opportunities/Monitor/Macro_Monitor.xlsx
+++ b/financial_models/Opportunities/Monitor/Macro_Monitor.xlsx
@@ -1,36 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kamanl/PycharmProjects/Invest_Proc/financial_models/Opportunities/Monitor/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerry chen\PycharmProjects\Invest_Proc\financial_models\Opportunities\Monitor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{832C731C-4746-4042-ABB1-D4F7608613AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5076E092-C1B4-47A5-98F6-AE05D64908A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="2940" windowWidth="16200" windowHeight="9300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3075" yWindow="1410" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Macro" sheetId="2" r:id="rId1"/>
     <sheet name="Analysis" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029" concurrentManualCount="8"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -332,7 +321,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -787,8 +776,8 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="超連結" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1072,19 +1061,19 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="2.5" customWidth="1"/>
-    <col min="2" max="2" width="62.5" customWidth="1"/>
-    <col min="3" max="3" width="10.5" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="32.6640625" customWidth="1"/>
-    <col min="5" max="5" width="10.5" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="32.6640625" customWidth="1"/>
-    <col min="7" max="7" width="10.5" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="32.6640625" customWidth="1"/>
+    <col min="1" max="1" width="2.42578125" customWidth="1"/>
+    <col min="2" max="2" width="62.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="32.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="32.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="32.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="15.75">
       <c r="A2" s="6"/>
       <c r="B2" s="5" t="s">
         <v>4</v>
@@ -1101,7 +1090,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="15.75">
       <c r="A3" s="11"/>
       <c r="B3" s="10" t="s">
         <v>2</v>
@@ -1119,7 +1108,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="15.75">
       <c r="A5" s="6"/>
       <c r="B5" s="5" t="s">
         <v>70</v>
@@ -1136,12 +1125,12 @@
         <v>HK</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8">
       <c r="B6" t="s">
         <v>71</v>
       </c>
       <c r="D6" s="1">
-        <v>4.7800000000000002E-2</v>
+        <v>4.3899999999999995E-2</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="1">
@@ -1149,15 +1138,15 @@
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="1">
-        <v>4.2069999999999996E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+        <v>4.3019999999999996E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="B7" s="44" t="s">
         <v>69</v>
       </c>
       <c r="D7" s="46">
-        <v>2.3199999999999998E-2</v>
+        <v>2.2200000000000001E-2</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="46">
@@ -1168,7 +1157,7 @@
         <v>1.5679999999999999E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="15.75">
       <c r="A9" s="6"/>
       <c r="B9" s="5" t="s">
         <v>73</v>
@@ -1185,7 +1174,7 @@
         <v>HK</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8">
       <c r="B10" t="s">
         <v>74</v>
       </c>
@@ -1201,7 +1190,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8">
       <c r="B12" s="48" t="s">
         <v>64</v>
       </c>
@@ -1212,7 +1201,7 @@
       <c r="E12" s="39"/>
       <c r="F12" s="47"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8">
       <c r="B13" s="48" t="s">
         <v>65</v>
       </c>
@@ -1226,7 +1215,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8">
       <c r="B14" s="48" t="s">
         <v>66</v>
       </c>
@@ -1263,17 +1252,17 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="2.5" customWidth="1"/>
-    <col min="2" max="2" width="62.5" customWidth="1"/>
-    <col min="3" max="3" width="10.5" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="32.6640625" customWidth="1"/>
-    <col min="5" max="5" width="10.5" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="32.6640625" customWidth="1"/>
+    <col min="1" max="1" width="2.42578125" customWidth="1"/>
+    <col min="2" max="2" width="62.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="32.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="32.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="15.75">
       <c r="A2" s="6"/>
       <c r="B2" s="5" t="s">
         <v>62</v>
@@ -1287,26 +1276,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="B3" t="s">
         <v>61</v>
       </c>
       <c r="D3" s="45">
         <f>Macro!D6-Macro!D7</f>
-        <v>2.4600000000000004E-2</v>
+        <v>2.1699999999999994E-2</v>
       </c>
       <c r="F3" s="45">
         <f>Macro!F6-Macro!F7</f>
         <v>7.9999999999999967E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="B4" s="44" t="s">
         <v>60</v>
       </c>
       <c r="D4" s="43">
         <f>D37</f>
-        <v>2.5520000000000001E-2</v>
+        <v>2.4420000000000004E-2</v>
       </c>
       <c r="E4" s="42"/>
       <c r="F4" s="41">
@@ -1314,7 +1303,7 @@
         <v>3.3600000000000005E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="B5" s="40" t="s">
         <v>59</v>
       </c>
@@ -1324,7 +1313,7 @@
       </c>
       <c r="D5" s="14">
         <f>SUM(D3:D4)</f>
-        <v>5.0120000000000005E-2</v>
+        <v>4.6119999999999994E-2</v>
       </c>
       <c r="E5" s="38">
         <f>IF(E29=4,1.2, IF(E29=-4,1.1,1))</f>
@@ -1335,7 +1324,7 @@
         <v>4.1599999999999998E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="15.75">
       <c r="A7" s="6"/>
       <c r="B7" s="37" t="s">
         <v>58</v>
@@ -1351,7 +1340,7 @@
         <v>China</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" s="11"/>
       <c r="B8" s="13" t="s">
         <v>57</v>
@@ -1361,7 +1350,7 @@
       <c r="E8" s="29"/>
       <c r="F8" s="33"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9" s="11"/>
       <c r="B9" s="29" t="s">
         <v>56</v>
@@ -1381,7 +1370,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10" s="11"/>
       <c r="B10" s="29" t="s">
         <v>54</v>
@@ -1401,7 +1390,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11" s="11"/>
       <c r="B11" s="29" t="s">
         <v>51</v>
@@ -1421,7 +1410,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12" s="11"/>
       <c r="B12" s="11" t="s">
         <v>49</v>
@@ -1441,7 +1430,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13" s="11"/>
       <c r="B13" s="27" t="s">
         <v>47</v>
@@ -1463,7 +1452,7 @@
         <v>Mixed</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14" s="11"/>
       <c r="B14" s="29" t="s">
         <v>46</v>
@@ -1483,7 +1472,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15" s="11"/>
       <c r="B15" s="29" t="s">
         <v>44</v>
@@ -1503,7 +1492,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16" s="11"/>
       <c r="B16" s="29" t="s">
         <v>42</v>
@@ -1523,7 +1512,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6">
       <c r="A17" s="11"/>
       <c r="B17" s="29" t="s">
         <v>40</v>
@@ -1543,7 +1532,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6">
       <c r="A18" s="11"/>
       <c r="B18" s="27" t="s">
         <v>38</v>
@@ -1565,7 +1554,7 @@
         <v>Cold</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6">
       <c r="A19" s="11"/>
       <c r="B19" s="29" t="s">
         <v>37</v>
@@ -1585,7 +1574,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6">
       <c r="A20" s="11"/>
       <c r="B20" s="29" t="s">
         <v>34</v>
@@ -1605,7 +1594,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6">
       <c r="A21" s="11"/>
       <c r="B21" s="29" t="s">
         <v>32</v>
@@ -1625,7 +1614,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6">
       <c r="A22" s="11"/>
       <c r="B22" s="29" t="s">
         <v>30</v>
@@ -1645,7 +1634,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6">
       <c r="A23" s="11"/>
       <c r="B23" s="27" t="s">
         <v>28</v>
@@ -1667,7 +1656,7 @@
         <v>Mixed</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6">
       <c r="A24" s="11"/>
       <c r="B24" s="29" t="s">
         <v>27</v>
@@ -1687,7 +1676,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6">
       <c r="A25" s="11"/>
       <c r="B25" s="29" t="s">
         <v>24</v>
@@ -1707,7 +1696,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6">
       <c r="A26" s="11"/>
       <c r="B26" s="29" t="s">
         <v>22</v>
@@ -1727,7 +1716,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6">
       <c r="A27" s="11"/>
       <c r="B27" s="29" t="s">
         <v>20</v>
@@ -1747,7 +1736,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6">
       <c r="A28" s="11"/>
       <c r="B28" s="27" t="s">
         <v>17</v>
@@ -1769,7 +1758,7 @@
         <v>Mixed</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6">
       <c r="A29" s="11"/>
       <c r="B29" s="24" t="s">
         <v>16</v>
@@ -1791,10 +1780,10 @@
         <v>Relatively pessimistic</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6">
       <c r="A30" s="11"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6">
       <c r="A31" s="11"/>
       <c r="B31" s="13" t="s">
         <v>15</v>
@@ -1808,7 +1797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6">
       <c r="A32" s="11"/>
       <c r="B32" s="11" t="s">
         <v>14</v>
@@ -1828,7 +1817,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:6">
       <c r="B33" s="11" t="s">
         <v>11</v>
       </c>
@@ -1849,7 +1838,7 @@
         <v>Mixed - Dormant</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:6">
       <c r="B34" s="11" t="s">
         <v>10</v>
       </c>
@@ -1870,7 +1859,7 @@
         <v>Hot - Positive</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:6">
       <c r="B35" s="11" t="s">
         <v>9</v>
       </c>
@@ -1891,7 +1880,7 @@
         <v>Mixed</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:6">
       <c r="B36" s="11" t="s">
         <v>8</v>
       </c>
@@ -1912,7 +1901,7 @@
         <v>Cold - Wide</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:6">
       <c r="B37" s="17" t="s">
         <v>7</v>
       </c>
@@ -1922,7 +1911,7 @@
       </c>
       <c r="D37" s="14">
         <f>Macro!D7*(1+C37)</f>
-        <v>2.5520000000000001E-2</v>
+        <v>2.4420000000000004E-2</v>
       </c>
       <c r="E37" s="15">
         <f>SUM(E32:E36)/10</f>
@@ -1933,12 +1922,12 @@
         <v>3.3600000000000005E-2</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:6">
       <c r="B39" s="13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:6">
       <c r="B40" t="s">
         <v>5</v>
       </c>

</xml_diff>